<commit_message>
ProductionLog is ready for testing API and Web
</commit_message>
<xml_diff>
--- a/public/assets/data/WeightData.xlsx
+++ b/public/assets/data/WeightData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\www\flock-sense\public\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085912DA-B9D1-4D6F-A16F-B83CFBDB8AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39C97FC-BFF9-44BA-A193-AAF321944571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -95,7 +95,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -405,7 +405,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add code for partners
</commit_message>
<xml_diff>
--- a/public/assets/data/WeightData.xlsx
+++ b/public/assets/data/WeightData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\www\flock-sense\public\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39C97FC-BFF9-44BA-A193-AAF321944571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADC2B05-4D25-496E-A5C2-71636D8DF775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -487,6 +487,17 @@
       </c>
       <c r="D6" s="3"/>
     </row>
+    <row r="7" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>45852</v>
+      </c>
+      <c r="B7" s="1">
+        <v>300</v>
+      </c>
+      <c r="C7" s="1">
+        <v>655900</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>